<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@bce5e0ea2125a7539a7dad36cc5fd0c09b756d54 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -3945,7 +3945,7 @@
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require individuals to be authenticated with an individual authenticator prior to using a group authenticator.</t>
+          <t>Red Hat Enterprise Linux 9must require individuals to be authenticated with an individual authenticator prior to using a group authenticator.</t>
         </is>
       </c>
       <c r="G50" s="2" t="inlineStr">
@@ -4999,7 +4999,7 @@
       </c>
       <c r="F65" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for network access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for network access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G65" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
       </c>
       <c r="F80" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for local access to privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for local access to privileged accounts.</t>
         </is>
       </c>
       <c r="G80" s="2" t="inlineStr">
@@ -6088,7 +6088,14 @@
         </is>
       </c>
       <c r="L80" s="2" t="n"/>
-      <c r="M80" s="2" t="inlineStr"/>
+      <c r="M80" s="2" t="inlineStr">
+        <is>
+          <t>To configure the system add or modify the following line in "/etc/ssh/sshd_config".
+PubkeyAuthentication yes
+Restart the SSH daemon for the settings to take effect:
+$ sudo systemctl restart sshd.service</t>
+        </is>
+      </c>
       <c r="N80" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -9410,7 +9417,7 @@
       </c>
       <c r="F129" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for local access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for local access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G129" s="2" t="inlineStr">
@@ -10979,7 +10986,7 @@
       </c>
       <c r="F151" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for network access to privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for network access to privileged accounts.</t>
         </is>
       </c>
       <c r="G151" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@0322da06cff4d5a92e264781ed0191091570fe5c 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -12820,7 +12820,7 @@
       </c>
       <c r="F181" s="2" t="inlineStr">
         <is>
-          <t>The operating system must isolate security functions from nonsecurity functions.</t>
+          <t>Red Hat Enterprise Linux 9 must isolate security functions from nonsecurity functions.</t>
         </is>
       </c>
       <c r="G181" s="2" t="inlineStr">
@@ -12864,7 +12864,16 @@
         </is>
       </c>
       <c r="L181" s="2" t="n"/>
-      <c r="M181" s="2" t="inlineStr"/>
+      <c r="M181" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To ensure that "vsyscall=none" is added as a kernel command line
+argument to newly installed kernels, add "vsyscall=none" to the
+default Grub2 command line for Linux operating systems.  Modify the line within
+"/etc/default/grub" as shown below:
+ GRUB_CMDLINE_LINUX="... vsyscall=none ..." 
+Run the following command to update command line for already installed kernels: # grubby --update-kernel=ALL --args="vsyscall=none" </t>
+        </is>
+      </c>
       <c r="N181" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@d44911404319a99b77eaba443d108b6e514c7778 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -642,7 +642,7 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>The operating system must manage excess capacity, bandwidth, or other redundancy to limit the effects of information flooding types of Denial of Service (DoS) attacks.</t>
+          <t>Red Hat Enterprise Linux 9 must manage excess capacity, bandwidth, or other redundancy to limit the effects of information flooding types of Denial of Service (DoS) attacks.</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
@@ -695,7 +695,15 @@
         </is>
       </c>
       <c r="L3" s="2" t="n"/>
-      <c r="M3" s="2" t="inlineStr"/>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to use TCP syncookies.
+Add or edit the following line in a system configuration file in the "/etc/sysctl.d/" directory:
+ net.ipv4.tcp_syncookies = 1
+ Load settings from all system configuration files with the following command:
+ $ sudo sysctl --system</t>
+        </is>
+      </c>
       <c r="N3" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@6f35897fdf463ee01c6a1e079f4ca6f4190e9c61 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -7701,7 +7701,7 @@
       </c>
       <c r="F103" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement replay-resistant authentication mechanisms for network access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 system must implement replay-resistant authentication mechanisms for network access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G103" s="2" t="inlineStr">
@@ -7715,7 +7715,7 @@
       <c r="H103" s="2" t="inlineStr"/>
       <c r="I103" s="2" t="inlineStr">
         <is>
-          <t>Applicable - Configurable</t>
+          <t>Applicable - Inherently Met</t>
         </is>
       </c>
       <c r="J103" s="2" t="inlineStr">
@@ -7723,17 +7723,36 @@
           <t>Verify the operating system implements replay-resistant authentication mechanisms for network access to non-privileged accounts. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K103" s="2" t="n"/>
+      <c r="K103" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 supports this requirement and cannot be configured to be out of compliance.
+Red Hat Enterprise Linux 9 inherently meets this requirement.</t>
+        </is>
+      </c>
       <c r="L103" s="2" t="n"/>
-      <c r="M103" s="2" t="n"/>
+      <c r="M103" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 inherently meets this requirement.
+No fix is required.</t>
+        </is>
+      </c>
       <c r="N103" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
         </is>
       </c>
       <c r="O103" s="2" t="n"/>
-      <c r="P103" s="2" t="n"/>
-      <c r="Q103" s="2" t="n"/>
+      <c r="P103" s="2" t="inlineStr">
+        <is>
+          <t>The release notes of OpenSSH 7.6 states "OpenSSH is a 100% complete SSH protocol 2.0 implementation and includes sftp client and server support."
+https://www.openssh.com/txt/release-7.6</t>
+        </is>
+      </c>
+      <c r="Q103" s="2" t="inlineStr">
+        <is>
+          <t>The OpenSSH package in Red Hat Enterprise Linux 9 is version 8.7, which is newer than 7.6 which only supports SSH protocol 2.0 which is restraint to replay attacks.</t>
+        </is>
+      </c>
     </row>
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@6602cecc7ce21c62273010f990712f3952d1b275 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -7505,7 +7505,7 @@
       </c>
       <c r="F100" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow the use of a temporary password for system logons with an immediate change to a permanent password.</t>
+          <t>Red Hat Enterprise Linux 9 must allow the use of a temporary password for system logons with an immediate change to a permanent password.</t>
         </is>
       </c>
       <c r="G100" s="2" t="inlineStr">
@@ -7514,10 +7514,17 @@
 Temporary passwords are typically used to allow access when new accounts are created or passwords are changed. It is common practice for administrators to create temporary passwords for user accounts which allow the users to log on, yet force them to change the password once they have successfully authenticated.</t>
         </is>
       </c>
-      <c r="H100" s="2" t="inlineStr"/>
+      <c r="H100" s="2" t="inlineStr">
+        <is>
+          <t>Without providing this capability, an account may be created without a password.
+Non-repudiation cannot be guaranteed once an account is created if a user is not forced to change the temporary password upon initial logon.
+Temporary passwords are typically used to allow access when new accounts are created or passwords are changed.
+It is common practice for administrators to create temporary passwords for user accounts that allow the users to log on, yet force them to change the password once they have successfully authenticated.</t>
+        </is>
+      </c>
       <c r="I100" s="2" t="inlineStr">
         <is>
-          <t>Applicable - Configurable</t>
+          <t>Applicable - Inherently Met</t>
         </is>
       </c>
       <c r="J100" s="2" t="inlineStr">
@@ -7525,7 +7532,12 @@
           <t>Verify the operating system allows the use of a temporary password for system logons with an immediate change to a permanent password. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K100" s="2" t="n"/>
+      <c r="K100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 supports this requirement and cannot be configured to be out of compliance.
+Red Hat Enterprise Linux 9 inherently meets this requirement.</t>
+        </is>
+      </c>
       <c r="L100" s="2" t="n"/>
       <c r="M100" s="2" t="n"/>
       <c r="N100" s="2" t="inlineStr">
@@ -7534,8 +7546,21 @@
         </is>
       </c>
       <c r="O100" s="2" t="n"/>
-      <c r="P100" s="2" t="n"/>
-      <c r="Q100" s="2" t="n"/>
+      <c r="P100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 offers the following commands to facilitate the use of a temporary password.
+chage -d 0 [username]
+(forces the user to change their password at next logon)
+passwd -e [username]
+(expires the passwd for a given user forcing a change at next logon.)</t>
+        </is>
+      </c>
+      <c r="Q100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 has the capability to perform temporary passwords based on organization policy.
+Configuration is not appropriate to define at an enterprise level.</t>
+        </is>
+      </c>
     </row>
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@fc94870f57cd0a23fdd3f300a0e2ac3751cf672d 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4, AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -621,7 +621,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, SC-5, SC-5 (2)</t>
+          <t>SC-5 (2),SC-5,CM-6 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (8), AC-6 (9), AU-12 (3), AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 b, AU-7 b, AU-8 b, AU-8 b, CM-5 (1)</t>
+          <t>AU-7 a,AC-6 (9),AU-8 b,AC-6 (8),CM-5 (1),AU-12 (3),AU-7 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b, AC-17 (1), AC-17 (9), CM-6 b, CM-6 b</t>
+          <t>AC-17 (9),CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11), IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1155,7 +1155,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b), CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1307,7 +1307,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b, AC-7 a</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>IA-2, IA-8, AU-3 (1)</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1596,7 +1596,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10), CM-6 b</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b), IA-5 (1) (a), IA-5 (1) (a), IA-5 (1) (a), IA-5 (1) (a), CM-6 b, IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e, SC-10, AC-12, MA-4 (7)</t>
+          <t>MA-4 (7),AC-12,SC-10,MA-4 e</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3, AU-3, AU-3, AU-3, AU-3 (1), AU-6 (4), AU-7 (1), AU-7 a, AU-14 (1), AU-3, CM-5 (1), MA-4 (1) (a), CM-6 b, AU-12 a, AU-7 a</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-7 a,AU-6 (4),AU-3,AU-12 a,CM-6 b,CM-5 (1),AU-14 (1),AU-7 (1)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2509,7 +2509,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8, SC-8 (1), SC-8 (2), SC-8 (2)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AU-3, AU-3 (1), AU-12 a, AC-2 (4), MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -2838,7 +2838,7 @@
     <row r="34" ht="130" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a, AC-11 b</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -3110,7 +3110,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9, SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3178,7 +3178,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3, CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3305,7 +3305,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1), AU-4 (1)</t>
+          <t>AU-4 (1)</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3377,7 +3377,7 @@
     <row r="42" ht="130" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1), SC-28, SC-28 (1)</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
@@ -3523,7 +3523,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>IA-11, IA-11, IA-11</t>
+          <t>IA-11</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3593,7 +3593,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a, AC-8 b, AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 b,AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3804,7 +3804,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, CM-6 b</t>
+          <t>CM-6 b</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -3932,7 +3932,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5), CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4140,7 +4140,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>SC-13, MA-4 (6), MA-4 (6)</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4277,7 +4277,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2), SC-8</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4348,7 +4348,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a), AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4835,7 +4835,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a, AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -4986,7 +4986,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2), CM-6 b, CM-6 b</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5126,7 +5126,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5252,7 +5252,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a, AU-12 (3), AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 b, AU-7 b, AU-8 b, AU-8 b, CM-5 (1), AU-12 c, AU-12 c, CM-6 b, AU-12 a</t>
+          <t>AU-7 a,AU-8 b,AU-12 a,CM-6 b,AU-12 c,CM-5 (1),AU-12 (3),AU-7 b</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5402,7 +5402,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-4 (1), AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5793,7 +5793,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AU-3, AU-3 (1), AU-12 a, AC-2 (4), MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -5958,7 +5958,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9, AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6029,7 +6029,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1), IA-2 (2), IA-2 (3), IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2 (4),IA-2 (1)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6116,7 +6116,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6449,7 +6449,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6595,7 +6595,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AC-6 (9), AU-12 c, CM-5 (1), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),CM-5 (1),AC-6 (9)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6662,7 +6662,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2, IA-2 (2), IA-2 (3), IA-2 (5), IA-2 (4)</t>
+          <t>IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (5),IA-2</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6742,7 +6742,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11), IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -6818,7 +6818,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7192,7 +7192,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1), AC-18 (1), SC-8 (1), SC-8</t>
+          <t>SC-8 (1),AC-18 (1),SC-8</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7268,7 +7268,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a), AU-8 (1) (b), AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7416,7 +7416,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9</t>
+          <t>AU-9</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -7565,7 +7565,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>IA-11, AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -7635,7 +7635,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8221,7 +8221,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a, AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -8763,7 +8763,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9053,7 +9053,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b, CM-7 a</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9123,7 +9123,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9193,7 +9193,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a, AC-18 (1)</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9378,7 +9378,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c), CM-7 a, CM-6 b</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -9940,7 +9940,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1), AC-11 b</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10161,7 +10161,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5), SI-6 b, SI-6 d</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10354,7 +10354,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (2), AC-2 (2)</t>
+          <t>AC-2 (2)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -10803,7 +10803,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-14 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c,AU-14 (1)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11364,7 +11364,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11496,7 +11496,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>SC-8, AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -12479,7 +12479,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>SI-16, CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -12851,7 +12851,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@abc17794fa6ca2816842712350eaf2004731d6c8 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -621,7 +621,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AC-6 (9),AU-8 b,AC-6 (8),CM-5 (1),AU-12 (3),AU-7 b</t>
+          <t>CM-5 (1),AU-7 b,AC-6 (9),AU-7 a,AC-6 (8),AU-12 (3),AU-8 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>AC-17 (9),CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1155,7 +1155,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>IA-8,AU-3 (1),IA-2</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1596,7 +1596,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),AC-12,SC-10,MA-4 e</t>
+          <t>MA-4 (7),SC-10,MA-4 e,AC-12</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-7 a,AU-6 (4),AU-3,AU-12 a,CM-6 b,CM-5 (1),AU-14 (1),AU-7 (1)</t>
+          <t>CM-5 (1),AU-6 (4),AU-3 (1),AU-7 a,AU-12 a,AU-7 (1),CM-6 b,AU-14 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2509,7 +2509,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -2838,7 +2838,7 @@
     <row r="34" ht="130" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -3178,7 +3178,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3439,7 +3439,13 @@
         </is>
       </c>
       <c r="L42" s="2" t="n"/>
-      <c r="M42" s="2" t="inlineStr"/>
+      <c r="M42" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to prevent unauthorized modification of all information at rest by using disk encryption.
+Encrypting a partition in an already installed system is more difficult, because existing partitions will need to be resized and changed.
+To encrypt an entire partition, dedicate a partition for encryption in the partition layout.</t>
+        </is>
+      </c>
       <c r="N42" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -3593,7 +3599,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 b,AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a,AC-8 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4140,7 +4146,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4348,7 +4354,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4986,7 +4992,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5126,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5252,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-8 b,AU-12 a,CM-6 b,AU-12 c,CM-5 (1),AU-12 (3),AU-7 b</t>
+          <t>CM-5 (1),AU-12 c,AU-7 b,AU-7 a,AU-12 a,CM-6 b,AU-12 (3),AU-8 b</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5402,7 +5408,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5793,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -5958,7 +5964,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6029,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2 (4),IA-2 (1)</t>
+          <t>IA-2 (3),IA-2 (2),IA-2 (1),IA-2 (4)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6116,7 +6122,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6449,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6595,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),CM-5 (1),AC-6 (9)</t>
+          <t>AU-12 c,CM-5 (1),AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6662,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (5),IA-2</t>
+          <t>IA-2 (2),IA-2 (3),IA-2 (5),IA-2,IA-2 (4)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6742,7 +6748,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -6818,7 +6824,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7192,7 +7198,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),AC-18 (1),SC-8</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7268,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7635,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8221,7 +8227,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -8763,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9123,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9378,7 +9384,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -9940,7 +9946,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10161,7 +10167,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 b,SI-6 d</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10803,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c,AU-14 (1)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-14 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11364,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12851,7 +12857,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -13673,7 +13679,7 @@
       </c>
       <c r="F192" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect the confidentiality and integrity of all information at rest.</t>
+          <t>Red Hat Enterprise Linux 9 must protect the confidentiality and integrity of all information at rest.</t>
         </is>
       </c>
       <c r="G192" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@53aed0d04952cc5f33f6c0970b48f9ffc7c3d198 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -621,7 +621,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5,SC-5 (2)</t>
+          <t>SC-5 (2),SC-5,CM-6 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-7 b,AC-6 (9),AU-7 a,AC-6 (8),AU-12 (3),AU-8 b</t>
+          <t>CM-5 (1),AC-6 (8),AU-12 (3),AU-7 b,AC-6 (9),AU-8 b,AU-7 a</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1155,7 +1155,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1307,7 +1307,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>IA-8,AU-3 (1),IA-2</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1596,7 +1596,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),SC-10,MA-4 e,AC-12</t>
+          <t>AC-12,MA-4 (7),MA-4 e,SC-10</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-6 (4),AU-3 (1),AU-7 a,AU-12 a,AU-7 (1),CM-6 b,AU-14 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,CM-5 (1),AU-7 (1),AU-14 (1),AU-12 a,AU-6 (4),MA-4 (1) (a),CM-6 b,AU-7 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2509,7 +2509,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -3377,7 +3377,7 @@
     <row r="42" ht="130" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4283,7 +4283,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4354,7 +4354,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4841,7 +4841,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5132,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5258,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c,AU-7 b,AU-7 a,AU-12 a,CM-6 b,AU-12 (3),AU-8 b</t>
+          <t>CM-5 (1),AU-12 (3),AU-7 b,AU-12 a,AU-8 b,AU-12 c,CM-6 b,AU-7 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5799,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6035,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (2),IA-2 (1),IA-2 (4)</t>
+          <t>IA-2 (4),IA-2 (3),IA-2 (2),IA-2 (1)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6122,7 +6122,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6455,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6601,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1),AC-2 (4),AC-6 (9)</t>
+          <t>CM-5 (1),AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6668,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2 (5),IA-2,IA-2 (4)</t>
+          <t>IA-2 (4),IA-2 (2),IA-2 (5),IA-2 (3),IA-2</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6748,7 +6748,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7274,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7571,7 +7571,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -7641,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8769,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9129,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9199,7 +9199,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -10167,7 +10167,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 b,SI-6 d</t>
+          <t>SI-6 b,CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10809,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-14 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-14 (1),AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11370,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11502,7 +11502,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -12857,7 +12857,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@2d18ba5a9ff660e66d0609c1fa719a520c5729ac 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -621,7 +621,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (8),AU-12 (3),AU-7 b,AC-6 (9),AU-8 b,AU-7 a</t>
+          <t>AU-7 a,AU-12 (3),AC-6 (9),AU-7 b,AU-8 b,CM-5 (1),AC-6 (8)</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (9),AC-17 (1)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1307,7 +1307,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1596,7 +1596,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 (7),MA-4 e,SC-10</t>
+          <t>MA-4 (7),SC-10,MA-4 e,AC-12</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-5 (1),AU-7 (1),AU-14 (1),AU-12 a,AU-6 (4),MA-4 (1) (a),CM-6 b,AU-7 a,AU-3 (1)</t>
+          <t>CM-6 b,AU-7 a,AU-3,AU-6 (4),AU-14 (1),AU-12 a,CM-5 (1),AU-7 (1),MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2509,7 +2509,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3 (1)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -3110,7 +3110,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3178,7 +3178,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3599,7 +3599,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a,AC-8 b</t>
+          <t>AC-8 a,AC-8 b,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4283,7 +4283,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4354,7 +4354,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4841,7 +4841,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5132,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5258,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 (3),AU-7 b,AU-12 a,AU-8 b,AU-12 c,CM-6 b,AU-7 a</t>
+          <t>CM-6 b,AU-7 a,AU-12 (3),AU-12 a,AU-7 b,AU-12 c,AU-8 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5799,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3 (1)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6035,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (3),IA-2 (2),IA-2 (1)</t>
+          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6122,7 +6122,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6455,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6601,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AC-6 (9),CM-5 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6668,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (5),IA-2 (3),IA-2</t>
+          <t>IA-2,IA-2 (3),IA-2 (2),IA-2 (5),IA-2 (4)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6748,7 +6748,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7198,7 +7198,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7274,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7641,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8227,7 +8227,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -8769,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9129,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9384,7 +9384,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10167,7 +10167,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10809,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-14 (1),AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-14 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11370,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11502,7 +11502,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -12485,7 +12485,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@b4ede572458fc0a3e3ca8f984e777ee7c2bf2ef6 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -621,7 +621,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5,SC-5 (2)</t>
+          <t>SC-5,SC-5 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-12 (3),AC-6 (9),AU-7 b,AU-8 b,CM-5 (1),AC-6 (8)</t>
+          <t>CM-5 (1),AC-6 (8),AU-7 b,AU-8 b,AU-12 (3),AU-7 a,AC-6 (9)</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (9),AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1155,7 +1155,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1307,7 +1307,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>IA-2,AU-3 (1),IA-8</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),SC-10,MA-4 e,AC-12</t>
+          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-7 a,AU-3,AU-6 (4),AU-14 (1),AU-12 a,CM-5 (1),AU-7 (1),MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-6 (4),AU-12 a,MA-4 (1) (a),AU-7 (1),AU-3,CM-5 (1),AU-3 (1),CM-6 b,AU-14 (1),AU-7 a</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1),AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-3,AC-2 (4),AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -3178,7 +3178,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3599,7 +3599,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 b,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 b,AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4354,7 +4354,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4992,7 +4992,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5132,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5258,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-7 a,AU-12 (3),AU-12 a,AU-7 b,AU-12 c,AU-8 b,CM-5 (1)</t>
+          <t>AU-12 a,CM-5 (1),AU-7 b,AU-8 b,AU-12 (3),CM-6 b,AU-7 a,AU-12 c</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5408,7 +5408,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5799,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1),AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-3,AC-2 (4),AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6035,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (1),IA-2 (2),IA-2 (3),IA-2 (4)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6122,7 +6122,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6455,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6601,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-6 (9),CM-5 (1),AC-2 (4)</t>
+          <t>AU-12 c,CM-5 (1),AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6668,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (3),IA-2 (2),IA-2 (5),IA-2 (4)</t>
+          <t>IA-2,IA-2 (4),IA-2 (5),IA-2 (2),IA-2 (3)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7198,7 +7198,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7274,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7641,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8769,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9059,7 +9059,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9129,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9199,7 +9199,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9384,7 +9384,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10809,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-14 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-14 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11370,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12485,7 +12485,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@75bb2908a7ea008345937532ce505a73de90940f 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -621,7 +621,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>SC-5 (2),SC-5,CM-6 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (8),AU-7 b,AU-8 b,AU-12 (3),AU-7 a,AC-6 (9)</t>
+          <t>AC-6 (9),AC-6 (8),AU-7 b,CM-5 (1),AU-7 a,AU-8 b,AU-12 (3)</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
+          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
+          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
+          <t>SC-10,MA-4 e,MA-4 (7),AC-12</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-12 a,MA-4 (1) (a),AU-7 (1),AU-3,CM-5 (1),AU-3 (1),CM-6 b,AU-14 (1),AU-7 a</t>
+          <t>CM-6 b,MA-4 (1) (a),AU-7 (1),AU-3,AU-14 (1),AU-3 (1),CM-5 (1),AU-7 a,AU-6 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2509,7 +2509,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AC-2 (4),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -3110,7 +3110,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3377,7 +3377,7 @@
     <row r="42" ht="130" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
@@ -3599,7 +3599,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 b,AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 b,AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4283,7 +4283,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -5132,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5258,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-5 (1),AU-7 b,AU-8 b,AU-12 (3),CM-6 b,AU-7 a,AU-12 c</t>
+          <t>AU-12 c,AU-7 b,CM-6 b,CM-5 (1),AU-7 a,AU-8 b,AU-12 a,AU-12 (3)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5799,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AC-2 (4),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -5964,7 +5964,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6035,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (2),IA-2 (3),IA-2 (4)</t>
+          <t>IA-2 (1),IA-2 (3),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6455,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6601,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1),AC-6 (9),AC-2 (4)</t>
+          <t>CM-5 (1),AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6668,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (4),IA-2 (5),IA-2 (2),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2,IA-2 (4),IA-2 (5)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6748,7 +6748,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -6824,7 +6824,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7198,7 +7198,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7274,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7571,7 +7571,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -7641,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8769,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9129,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9199,7 +9199,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9384,7 +9384,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -9946,7 +9946,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10167,7 +10167,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5),SI-6 b</t>
+          <t>SI-6 b,CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10809,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-14 (1),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-14 (1),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11370,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11502,7 +11502,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ComplianceAsCode/content@fe68fcd788b85eed7559e6174d71a676223ab02b 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-6 (8),AU-7 b,CM-5 (1),AU-7 a,AU-8 b,AU-12 (3)</t>
+          <t>AU-7 a,AU-12 (3),AC-6 (9),AU-7 b,CM-5 (1),AU-8 b,AC-6 (8)</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>CM-7 b,AC-17 (1),AC-17 (9),CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1155,7 +1155,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>IA-2,IA-8,AU-3 (1)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1596,7 +1596,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>SC-10,MA-4 e,MA-4 (7),AC-12</t>
+          <t>AC-12,MA-4 (7),MA-4 e,SC-10</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,MA-4 (1) (a),AU-7 (1),AU-3,AU-14 (1),AU-3 (1),CM-5 (1),AU-7 a,AU-6 (4),AU-12 a</t>
+          <t>AU-7 a,AU-6 (4),AU-3,AU-3 (1),AU-7 (1),CM-5 (1),MA-4 (1) (a),AU-12 a,AU-14 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2509,7 +2509,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -3178,7 +3178,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3599,7 +3599,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 b,AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 b,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4841,7 +4841,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -4992,7 +4992,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5132,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5258,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-7 b,CM-6 b,CM-5 (1),AU-7 a,AU-8 b,AU-12 a,AU-12 (3)</t>
+          <t>AU-12 (3),AU-7 a,AU-7 b,CM-5 (1),AU-8 b,AU-12 a,AU-12 c,CM-6 b</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5799,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -5964,7 +5964,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6035,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (3),IA-2 (2),IA-2 (4)</t>
+          <t>IA-2 (3),IA-2 (1),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6455,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6601,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AC-2 (4),AU-12 c,CM-5 (1),AC-6 (9)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6668,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2,IA-2 (4),IA-2 (5)</t>
+          <t>IA-2,IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (5)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6824,7 +6824,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7198,7 +7198,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7274,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7641,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8769,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9059,7 +9059,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9129,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9199,7 +9199,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9384,7 +9384,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -9946,7 +9946,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10167,7 +10167,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,CM-3 (5),SI-6 d</t>
+          <t>CM-3 (5),SI-6 d,SI-6 b</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10809,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-14 (1),AU-3 (1),AU-12 a</t>
+          <t>AU-14 (1),AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11370,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">

</xml_diff>